<commit_message>
update cd e isd
</commit_message>
<xml_diff>
--- a/AulasT_Arq/praticas/P06-results-alunos.xlsx
+++ b/AulasT_Arq/praticas/P06-results-alunos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t xml:space="preserve">gemm5()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
   </si>
 </sst>
 </file>
@@ -470,13 +473,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.24"/>
@@ -533,61 +536,91 @@
         <v>8</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="6" t="n">
+        <v>403</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>1073</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="6" t="n">
+        <v>401</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>671</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="C6" s="11" t="n">
+        <v>208</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>671</v>
+      </c>
+      <c r="E6" s="11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="C7" s="11" t="n">
+        <v>111</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>469</v>
+      </c>
+      <c r="E7" s="11" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="C8" s="11" t="n">
+        <v>110</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>301</v>
+      </c>
+      <c r="E8" s="11" t="n">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="13" t="e">
+      <c r="C9" s="13" t="n">
         <f aca="false">C5/C8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D9" s="13" t="e">
+        <v>3.64545454545455</v>
+      </c>
+      <c r="D9" s="13" t="n">
         <f aca="false">D5/D8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E9" s="13" t="e">
+        <v>2.22923588039867</v>
+      </c>
+      <c r="E9" s="13" t="n">
         <f aca="false">E5/E8</f>
-        <v>#DIV/0!</v>
+        <v>1.66666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -655,6 +688,11 @@
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>